<commit_message>
more updates for dairy/beef
</commit_message>
<xml_diff>
--- a/SG_Ag_compendium/Data/beef_sector.xlsx
+++ b/SG_Ag_compendium/Data/beef_sector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z620777\OneDrive - SCOTS Connect\R\SG_Ag_compendium\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/jacqueline_massaya_gov_scot/Documents/R/SG_ag_comp/SG_Ag_compendium/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D076C52B-5D06-4828-899B-32EBC355A613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D076C52B-5D06-4828-899B-32EBC355A613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F445AD0A-00B4-46E2-9768-455830E76379}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{A31DD5EF-659B-45FE-9B3B-99211DD7E9DA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A31DD5EF-659B-45FE-9B3B-99211DD7E9DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,7 +435,7 @@
         <v>409213</v>
       </c>
       <c r="D2">
-        <v>394709</v>
+        <v>394698</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -449,7 +449,7 @@
         <v>8330</v>
       </c>
       <c r="D3">
-        <v>8134</v>
+        <v>8127</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>